<commit_message>
Update Hingga Rabu Pagi
</commit_message>
<xml_diff>
--- a/storage/app/public/template_upload/Format_Upload_Putus_Sekolah.xlsx
+++ b/storage/app/public/template_upload/Format_Upload_Putus_Sekolah.xlsx
@@ -377,7 +377,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -645,6 +645,12 @@
       </c>
       <c r="G9">
         <v>5</v>
+      </c>
+      <c r="H9">
+        <v>67</v>
+      </c>
+      <c r="I9">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>